<commit_message>
update kiem tra ds
</commit_message>
<xml_diff>
--- a/DSSV_Test.xlsx
+++ b/DSSV_Test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Test_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B50ECC9-14B4-4D2C-A0ED-B87EC1596AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B16221FB-FAB5-4AED-8B58-D931C4144DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1335" yWindow="3870" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>STT</t>
   </si>
@@ -59,6 +59,30 @@
   </si>
   <si>
     <t>Nơ</t>
+  </si>
+  <si>
+    <t>N22DCPT032</t>
+  </si>
+  <si>
+    <t>Văn</t>
+  </si>
+  <si>
+    <t>Từng</t>
+  </si>
+  <si>
+    <t>D22CNQ01-T</t>
+  </si>
+  <si>
+    <t>N21DCPT02</t>
+  </si>
+  <si>
+    <t>Đinh</t>
+  </si>
+  <si>
+    <t>Oanh</t>
+  </si>
+  <si>
+    <t>D21CPPT-M</t>
   </si>
 </sst>
 </file>
@@ -421,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +533,66 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>